<commit_message>
Network State Manager Added with Code Clean Up
</commit_message>
<xml_diff>
--- a/test/input_data/TriangleNetworkData.xlsx
+++ b/test/input_data/TriangleNetworkData.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Documents\GitHub\Webslinger\test\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DC1BE9-59F2-472E-BA69-45C2A492F5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE9F0D1-FFB4-48EC-BB83-C076D1A1A371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="15276" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TriangleData" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>N_ID</t>
   </si>
@@ -93,10 +94,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -316,10 +323,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -327,10 +334,11 @@
     <col min="1" max="1" width="21.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="12.5703125" style="1"/>
+    <col min="4" max="4" width="30.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="12.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -341,62 +349,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -404,161 +412,387 @@
         <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C8" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="C9" s="1">
+      <c r="B10" s="1">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3">
         <v>3</v>
       </c>
-      <c r="B11" s="1" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3">
         <v>4</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
+    </row>
+    <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>6</v>
+      </c>
+      <c r="B21" s="3">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>7</v>
+      </c>
+      <c r="B22" s="3">
+        <v>7</v>
+      </c>
+      <c r="C22" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>8</v>
+      </c>
+      <c r="B23" s="3">
+        <v>8</v>
+      </c>
+      <c r="C23" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>9</v>
+      </c>
+      <c r="B24" s="3">
+        <v>9</v>
+      </c>
+      <c r="C24" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>10</v>
+      </c>
+      <c r="B25" s="3">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>11</v>
+      </c>
+      <c r="B26" s="3">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>12</v>
+      </c>
+      <c r="B27" s="3">
+        <v>5</v>
+      </c>
+      <c r="C27" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>13</v>
+      </c>
+      <c r="B28" s="3">
+        <v>11</v>
+      </c>
+      <c r="C28" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>14</v>
+      </c>
+      <c r="B29" s="3">
+        <v>12</v>
+      </c>
+      <c r="C29" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>15</v>
+      </c>
+      <c r="B30" s="3">
+        <v>6</v>
+      </c>
+      <c r="C30" s="3">
         <v>1</v>
       </c>
-      <c r="B12" s="1">
+    </row>
+    <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>16</v>
+      </c>
+      <c r="B31" s="3">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>17</v>
+      </c>
+      <c r="B32" s="3">
+        <v>8</v>
+      </c>
+      <c r="C32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>18</v>
+      </c>
+      <c r="B33" s="3">
+        <v>10</v>
+      </c>
+      <c r="C33" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>19</v>
+      </c>
+      <c r="B34" s="3">
+        <v>11</v>
+      </c>
+      <c r="C34" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>20</v>
+      </c>
+      <c r="B35" s="3">
+        <v>12</v>
+      </c>
+      <c r="C35" s="3">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1">
-        <v>2</v>
-      </c>
-      <c r="C14" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1">
-        <v>3</v>
-      </c>
-      <c r="C15" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1">
-        <v>4</v>
-      </c>
-      <c r="C16" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+    </row>
+    <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="1">
-        <v>5</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="B37" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B14">
+    <sortCondition descending="1" ref="B2:B14"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EE4C83-22AE-400D-B87E-E614C1B0850A}">
+  <dimension ref="G21:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G21" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="H21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="1">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="1">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="1">
+    <row r="23" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="1">
         <v>1400</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify And Export Network Implemented
</commit_message>
<xml_diff>
--- a/test/input_data/TriangleNetworkData.xlsx
+++ b/test/input_data/TriangleNetworkData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Logan\Documents\GitHub\Webslinger\test\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE9F0D1-FFB4-48EC-BB83-C076D1A1A371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A623180-464E-44FF-9A5F-58C59A6E6993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="12960" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TriangleData" sheetId="2" r:id="rId1"/>
@@ -21,25 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
-  <si>
-    <t>N_ID</t>
-  </si>
-  <si>
-    <t>N_X</t>
-  </si>
-  <si>
-    <t>N_Y</t>
-  </si>
-  <si>
-    <t>E_ID</t>
-  </si>
-  <si>
-    <t>N_FROM</t>
-  </si>
-  <si>
-    <t>N_TO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>META_NET_PROP</t>
   </si>
@@ -60,6 +42,30 @@
   </si>
   <si>
     <t>static</t>
+  </si>
+  <si>
+    <t>n_id</t>
+  </si>
+  <si>
+    <t>n_x</t>
+  </si>
+  <si>
+    <t>n_y</t>
+  </si>
+  <si>
+    <t>e_id</t>
+  </si>
+  <si>
+    <t>n_from</t>
+  </si>
+  <si>
+    <t>n_to</t>
+  </si>
+  <si>
+    <t>meta_key</t>
+  </si>
+  <si>
+    <t>meta_value</t>
   </si>
 </sst>
 </file>
@@ -325,8 +331,8 @@
   </sheetPr>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -340,13 +346,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -484,13 +490,13 @@
     <row r="14" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
@@ -716,23 +722,23 @@
     <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B39" s="1">
         <v>1400</v>
@@ -740,10 +746,10 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -766,23 +772,23 @@
   <sheetData>
     <row r="21" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G21" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G22" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G23" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H23" s="1">
         <v>1400</v>
@@ -790,10 +796,10 @@
     </row>
     <row r="24" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G24" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>